<commit_message>
Iniciar el dia de 15-10-2019 se ha modificado el diseño
</commit_message>
<xml_diff>
--- a/app/model/reportes/Reporte.xlsx
+++ b/app/model/reportes/Reporte.xlsx
@@ -15,9 +15,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="7">
-  <si>
-    <t>Reporte generado: 2019-10-11 15:29:57</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="12">
+  <si>
+    <t>Reporte generado: 2019-10-12 08:56:57</t>
   </si>
   <si>
     <t>MONITOREO DE USUARIOS</t>
@@ -36,6 +36,21 @@
   </si>
   <si>
     <t>ESTADO</t>
+  </si>
+  <si>
+    <t>CARTAGO</t>
+  </si>
+  <si>
+    <t>SEDE1</t>
+  </si>
+  <si>
+    <t>JESUS CAMARA</t>
+  </si>
+  <si>
+    <t>2019-10-12 08:56:51</t>
+  </si>
+  <si>
+    <t>CONECTADO</t>
   </si>
 </sst>
 </file>
@@ -63,7 +78,7 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -76,6 +91,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="C8C8C8"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="45A236"/>
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
@@ -100,7 +121,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
@@ -108,6 +129,12 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
     <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="0">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="0">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="3" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="0">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
   </cellXfs>
@@ -409,19 +436,19 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A4" sqref="A4:E4"/>
+      <selection activeCell="A4" sqref="A4:E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="8.140869" bestFit="true" customWidth="true" style="0"/>
-    <col min="2" max="2" width="5.855713" bestFit="true" customWidth="true" style="0"/>
-    <col min="3" max="3" width="9.283447" bestFit="true" customWidth="true" style="0"/>
-    <col min="4" max="4" width="6.998291" bestFit="true" customWidth="true" style="0"/>
-    <col min="5" max="5" width="8.140869" bestFit="true" customWidth="true" style="0"/>
+    <col min="1" max="1" width="9.283447" bestFit="true" customWidth="true" style="0"/>
+    <col min="2" max="2" width="6.998291" bestFit="true" customWidth="true" style="0"/>
+    <col min="3" max="3" width="15.281982" bestFit="true" customWidth="true" style="0"/>
+    <col min="4" max="4" width="23.422852" bestFit="true" customWidth="true" style="0"/>
+    <col min="5" max="5" width="11.711426" bestFit="true" customWidth="true" style="0"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -449,6 +476,23 @@
       </c>
       <c r="E4" s="2" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Termino el dia 2019-10-15 se realizo validaciones en modulo de Configuracion de usuarios y seguridad en los modulos.
</commit_message>
<xml_diff>
--- a/app/model/reportes/Reporte.xlsx
+++ b/app/model/reportes/Reporte.xlsx
@@ -15,9 +15,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="12">
-  <si>
-    <t>Reporte generado: 2019-10-12 08:56:57</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="16">
+  <si>
+    <t>Reporte generado: 2019-10-15 15:35:31</t>
   </si>
   <si>
     <t>MONITOREO DE USUARIOS</t>
@@ -38,19 +38,31 @@
     <t>ESTADO</t>
   </si>
   <si>
-    <t>CARTAGO</t>
-  </si>
-  <si>
-    <t>SEDE1</t>
+    <t>PEREIRA</t>
+  </si>
+  <si>
+    <t>SEDEPEREIRA1</t>
+  </si>
+  <si>
+    <t>ELISA</t>
+  </si>
+  <si>
+    <t>2019-10-15 13:15:54</t>
+  </si>
+  <si>
+    <t>DESCONECTADO</t>
+  </si>
+  <si>
+    <t>CAMILACAMARA</t>
+  </si>
+  <si>
+    <t>2019-10-15 13:22:07</t>
   </si>
   <si>
     <t>JESUS CAMARA</t>
   </si>
   <si>
-    <t>2019-10-12 08:56:51</t>
-  </si>
-  <si>
-    <t>CONECTADO</t>
+    <t>2019-10-15 13:22:32</t>
   </si>
 </sst>
 </file>
@@ -78,7 +90,7 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -96,7 +108,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="45A236"/>
+        <fgColor rgb="F2F2F2"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="D53737"/>
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
@@ -121,7 +139,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
@@ -135,6 +153,9 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
     <xf xfId="0" fontId="0" numFmtId="0" fillId="3" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="0">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="4" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="0">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
   </cellXfs>
@@ -436,19 +457,19 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A4" sqref="A4:E5"/>
+      <selection activeCell="A4" sqref="A4:E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="1" width="9.283447" bestFit="true" customWidth="true" style="0"/>
-    <col min="2" max="2" width="6.998291" bestFit="true" customWidth="true" style="0"/>
+    <col min="2" max="2" width="15.281982" bestFit="true" customWidth="true" style="0"/>
     <col min="3" max="3" width="15.281982" bestFit="true" customWidth="true" style="0"/>
     <col min="4" max="4" width="23.422852" bestFit="true" customWidth="true" style="0"/>
-    <col min="5" max="5" width="11.711426" bestFit="true" customWidth="true" style="0"/>
+    <col min="5" max="5" width="15.281982" bestFit="true" customWidth="true" style="0"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -491,7 +512,41 @@
       <c r="D5" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" s="5" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>

<commit_message>
modificaciones mejora de seguridad recuperar empresa completa cambio de reportes Finalizacion de Proyecto
</commit_message>
<xml_diff>
--- a/app/model/reportes/Reporte.xlsx
+++ b/app/model/reportes/Reporte.xlsx
@@ -15,9 +15,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="16">
-  <si>
-    <t>Reporte generado: 2019-10-15 15:35:31</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="12">
+  <si>
+    <t>Reporte generado: 2019-10-16 11:49:42</t>
   </si>
   <si>
     <t>MONITOREO DE USUARIOS</t>
@@ -38,31 +38,19 @@
     <t>ESTADO</t>
   </si>
   <si>
-    <t>PEREIRA</t>
-  </si>
-  <si>
-    <t>SEDEPEREIRA1</t>
-  </si>
-  <si>
-    <t>ELISA</t>
-  </si>
-  <si>
-    <t>2019-10-15 13:15:54</t>
-  </si>
-  <si>
-    <t>DESCONECTADO</t>
-  </si>
-  <si>
-    <t>CAMILACAMARA</t>
-  </si>
-  <si>
-    <t>2019-10-15 13:22:07</t>
-  </si>
-  <si>
-    <t>JESUS CAMARA</t>
-  </si>
-  <si>
-    <t>2019-10-15 13:22:32</t>
+    <t>CARTAGO</t>
+  </si>
+  <si>
+    <t>SEDE INGETRONIK</t>
+  </si>
+  <si>
+    <t>YISUS</t>
+  </si>
+  <si>
+    <t>2019-10-16 11:49:42</t>
+  </si>
+  <si>
+    <t>CONECTADO</t>
   </si>
 </sst>
 </file>
@@ -90,7 +78,7 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -108,13 +96,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="F2F2F2"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="D53737"/>
+        <fgColor rgb="45A236"/>
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
@@ -139,7 +121,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
@@ -153,9 +135,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
     <xf xfId="0" fontId="0" numFmtId="0" fillId="3" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="4" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="0">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
   </cellXfs>
@@ -457,19 +436,19 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A4" sqref="A4:E7"/>
+      <selection activeCell="A4" sqref="A4:E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="1" width="9.283447" bestFit="true" customWidth="true" style="0"/>
-    <col min="2" max="2" width="15.281982" bestFit="true" customWidth="true" style="0"/>
-    <col min="3" max="3" width="15.281982" bestFit="true" customWidth="true" style="0"/>
+    <col min="2" max="2" width="18.709717" bestFit="true" customWidth="true" style="0"/>
+    <col min="3" max="3" width="9.283447" bestFit="true" customWidth="true" style="0"/>
     <col min="4" max="4" width="23.422852" bestFit="true" customWidth="true" style="0"/>
-    <col min="5" max="5" width="15.281982" bestFit="true" customWidth="true" style="0"/>
+    <col min="5" max="5" width="11.711426" bestFit="true" customWidth="true" style="0"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -512,41 +491,7 @@
       <c r="D5" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E7" s="5" t="s">
+      <c r="E5" s="4" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>